<commit_message>
changed model structure and local batch size
</commit_message>
<xml_diff>
--- a/Data/results.xlsx
+++ b/Data/results.xlsx
@@ -402,10 +402,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>15.34749794006348</v>
+        <v>52.40544891357422</v>
       </c>
       <c r="C2">
-        <v>-0.09871423244476318</v>
+        <v>-8.547795295715332</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -413,10 +413,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>9.904510498046875</v>
+        <v>46.81840896606445</v>
       </c>
       <c r="C3">
-        <v>0.5143470764160156</v>
+        <v>-6.757501602172852</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -424,10 +424,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>8.556663513183594</v>
+        <v>34.35824203491211</v>
       </c>
       <c r="C4">
-        <v>0.6386956572532654</v>
+        <v>-3.568210124969482</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -435,10 +435,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7.894490718841553</v>
+        <v>17.29892349243164</v>
       </c>
       <c r="C5">
-        <v>0.6941730976104736</v>
+        <v>-0.4281232357025146</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -446,10 +446,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7.065867900848389</v>
+        <v>14.36217784881592</v>
       </c>
       <c r="C6">
-        <v>0.7525091171264648</v>
+        <v>0.01025795936584473</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -457,10 +457,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>7.00786828994751</v>
+        <v>13.10221481323242</v>
       </c>
       <c r="C7">
-        <v>0.7519485354423523</v>
+        <v>0.1583518385887146</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -468,10 +468,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>6.826406955718994</v>
+        <v>11.9117431640625</v>
       </c>
       <c r="C8">
-        <v>0.7706104516983032</v>
+        <v>0.2958714365959167</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -479,10 +479,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>6.560525417327881</v>
+        <v>11.88819599151611</v>
       </c>
       <c r="C9">
-        <v>0.7804350852966309</v>
+        <v>0.2927542924880981</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -490,10 +490,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>6.286630630493164</v>
+        <v>11.46057510375977</v>
       </c>
       <c r="C10">
-        <v>0.7965658903121948</v>
+        <v>0.3718902468681335</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -501,10 +501,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>6.319224834442139</v>
+        <v>10.67667865753174</v>
       </c>
       <c r="C11">
-        <v>0.8003485202789307</v>
+        <v>0.420953094959259</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -512,10 +512,10 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>6.32938814163208</v>
+        <v>10.54313182830811</v>
       </c>
       <c r="C12">
-        <v>0.8010615110397339</v>
+        <v>0.4576348662376404</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -523,10 +523,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5.833780765533447</v>
+        <v>10.17471218109131</v>
       </c>
       <c r="C13">
-        <v>0.8256620168685913</v>
+        <v>0.4804003238677979</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -534,10 +534,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>5.902934551239014</v>
+        <v>9.824414253234863</v>
       </c>
       <c r="C14">
-        <v>0.8219512104988098</v>
+        <v>0.5154540538787842</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -545,10 +545,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>5.765151023864746</v>
+        <v>9.503444671630859</v>
       </c>
       <c r="C15">
-        <v>0.8233551979064941</v>
+        <v>0.5291653871536255</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -556,10 +556,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>5.784880638122559</v>
+        <v>9.515039443969727</v>
       </c>
       <c r="C16">
-        <v>0.8267849087715149</v>
+        <v>0.5458121299743652</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -567,10 +567,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>5.659507751464844</v>
+        <v>8.62856388092041</v>
       </c>
       <c r="C17">
-        <v>0.8327701687812805</v>
+        <v>0.6253806352615356</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -578,10 +578,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>5.461693286895752</v>
+        <v>8.494733810424805</v>
       </c>
       <c r="C18">
-        <v>0.8509398102760315</v>
+        <v>0.641605019569397</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -589,10 +589,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>5.316556453704834</v>
+        <v>8.588038444519043</v>
       </c>
       <c r="C19">
-        <v>0.851973831653595</v>
+        <v>0.6405611634254456</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -600,10 +600,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>5.461806774139404</v>
+        <v>8.093818664550781</v>
       </c>
       <c r="C20">
-        <v>0.8469261527061462</v>
+        <v>0.6663030385971069</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -611,10 +611,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>5.270605087280273</v>
+        <v>8.45398998260498</v>
       </c>
       <c r="C21">
-        <v>0.8571687340736389</v>
+        <v>0.6373758316040039</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -622,10 +622,10 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>5.242054462432861</v>
+        <v>8.554228782653809</v>
       </c>
       <c r="C22">
-        <v>0.8618252873420715</v>
+        <v>0.6307522058486938</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -633,10 +633,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>5.266852378845215</v>
+        <v>7.638081073760986</v>
       </c>
       <c r="C23">
-        <v>0.8498634099960327</v>
+        <v>0.6969456672668457</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -644,10 +644,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>5.175135135650635</v>
+        <v>7.551326274871826</v>
       </c>
       <c r="C24">
-        <v>0.865251898765564</v>
+        <v>0.7162183523178101</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -655,10 +655,10 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>5.180182933807373</v>
+        <v>7.465870380401611</v>
       </c>
       <c r="C25">
-        <v>0.8587640523910522</v>
+        <v>0.7159451842308044</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -666,10 +666,10 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>5.299636363983154</v>
+        <v>7.51484489440918</v>
       </c>
       <c r="C26">
-        <v>0.8547170758247375</v>
+        <v>0.7141540050506592</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -677,10 +677,10 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>5.246651649475098</v>
+        <v>7.385990142822266</v>
       </c>
       <c r="C27">
-        <v>0.8551961183547974</v>
+        <v>0.7066656351089478</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -688,10 +688,10 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>4.972257614135742</v>
+        <v>7.148406982421875</v>
       </c>
       <c r="C28">
-        <v>0.8713397979736328</v>
+        <v>0.7444168329238892</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -699,10 +699,10 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>5.047584533691406</v>
+        <v>7.007951259613037</v>
       </c>
       <c r="C29">
-        <v>0.869644820690155</v>
+        <v>0.7345058917999268</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -710,10 +710,10 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>5.06443977355957</v>
+        <v>7.092115879058838</v>
       </c>
       <c r="C30">
-        <v>0.8671430349349976</v>
+        <v>0.7381138205528259</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -721,10 +721,10 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>5.306185722351074</v>
+        <v>7.044261932373047</v>
       </c>
       <c r="C31">
-        <v>0.8477938771247864</v>
+        <v>0.7389810085296631</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -732,10 +732,10 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>4.85390043258667</v>
+        <v>7.078729629516602</v>
       </c>
       <c r="C32">
-        <v>0.8781085014343262</v>
+        <v>0.7300344705581665</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -743,10 +743,10 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>4.976870059967041</v>
+        <v>6.744141578674316</v>
       </c>
       <c r="C33">
-        <v>0.8744519948959351</v>
+        <v>0.7561941146850586</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -754,10 +754,10 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>4.939432144165039</v>
+        <v>6.728821754455566</v>
       </c>
       <c r="C34">
-        <v>0.8728706240653992</v>
+        <v>0.7592419981956482</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -765,10 +765,10 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>5.149592876434326</v>
+        <v>6.586283206939697</v>
       </c>
       <c r="C35">
-        <v>0.8651048541069031</v>
+        <v>0.780877947807312</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -776,10 +776,10 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>4.831544399261475</v>
+        <v>6.427896499633789</v>
       </c>
       <c r="C36">
-        <v>0.8782818913459778</v>
+        <v>0.7780163884162903</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -787,10 +787,10 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>4.899415493011475</v>
+        <v>6.432909965515137</v>
       </c>
       <c r="C37">
-        <v>0.8719736337661743</v>
+        <v>0.7741916179656982</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -798,10 +798,10 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>4.94515323638916</v>
+        <v>6.603747844696045</v>
       </c>
       <c r="C38">
-        <v>0.8725342750549316</v>
+        <v>0.7715558409690857</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -809,10 +809,10 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>4.884621143341064</v>
+        <v>6.33154821395874</v>
       </c>
       <c r="C39">
-        <v>0.8792588114738464</v>
+        <v>0.7899177670478821</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -820,10 +820,10 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>4.967241764068604</v>
+        <v>6.084758758544922</v>
       </c>
       <c r="C40">
-        <v>0.8740785121917725</v>
+        <v>0.8082225322723389</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -831,10 +831,10 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>4.779223442077637</v>
+        <v>6.289232730865479</v>
       </c>
       <c r="C41">
-        <v>0.8823297619819641</v>
+        <v>0.7875809669494629</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -842,10 +842,10 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>4.707613468170166</v>
+        <v>6.236540794372559</v>
       </c>
       <c r="C42">
-        <v>0.8876652121543884</v>
+        <v>0.7956802248954773</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -853,10 +853,10 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>4.816047668457031</v>
+        <v>6.089844703674316</v>
       </c>
       <c r="C43">
-        <v>0.8845153450965881</v>
+        <v>0.8005338907241821</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -864,10 +864,10 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>4.512068748474121</v>
+        <v>6.340396404266357</v>
       </c>
       <c r="C44">
-        <v>0.8909177184104919</v>
+        <v>0.7857683897018433</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -875,10 +875,10 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>4.547167778015137</v>
+        <v>6.036722660064697</v>
       </c>
       <c r="C45">
-        <v>0.8903572559356689</v>
+        <v>0.8039543628692627</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -886,10 +886,10 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>4.794087886810303</v>
+        <v>5.884133338928223</v>
       </c>
       <c r="C46">
-        <v>0.8823930025100708</v>
+        <v>0.8104521632194519</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -897,10 +897,10 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>4.790929794311523</v>
+        <v>5.972614288330078</v>
       </c>
       <c r="C47">
-        <v>0.8828291893005371</v>
+        <v>0.8177534341812134</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -908,10 +908,10 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>4.76503324508667</v>
+        <v>5.968766212463379</v>
       </c>
       <c r="C48">
-        <v>0.8816277384757996</v>
+        <v>0.8072613477706909</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -919,10 +919,10 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>4.744868278503418</v>
+        <v>5.956734657287598</v>
       </c>
       <c r="C49">
-        <v>0.8855288624763489</v>
+        <v>0.8082748651504517</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -930,10 +930,10 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>4.537713527679443</v>
+        <v>6.048097133636475</v>
       </c>
       <c r="C50">
-        <v>0.8960544466972351</v>
+        <v>0.8112385869026184</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -941,10 +941,10 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>4.600777626037598</v>
+        <v>5.791770458221436</v>
       </c>
       <c r="C51">
-        <v>0.8918130993843079</v>
+        <v>0.8219859600067139</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -952,10 +952,10 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>4.762045383453369</v>
+        <v>5.844794273376465</v>
       </c>
       <c r="C52">
-        <v>0.8848091959953308</v>
+        <v>0.8207231760025024</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -963,10 +963,10 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>4.639951229095459</v>
+        <v>5.726579666137695</v>
       </c>
       <c r="C53">
-        <v>0.8847997188568115</v>
+        <v>0.8211728930473328</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -974,10 +974,10 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>4.795880317687988</v>
+        <v>5.759580135345459</v>
       </c>
       <c r="C54">
-        <v>0.8802478313446045</v>
+        <v>0.8164608478546143</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -985,10 +985,10 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>4.774169921875</v>
+        <v>5.86553430557251</v>
       </c>
       <c r="C55">
-        <v>0.8815128803253174</v>
+        <v>0.8184210062026978</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -996,10 +996,10 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>4.588617324829102</v>
+        <v>5.660834789276123</v>
       </c>
       <c r="C56">
-        <v>0.8896726369857788</v>
+        <v>0.8300696611404419</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1007,10 +1007,10 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>4.712937355041504</v>
+        <v>5.815227031707764</v>
       </c>
       <c r="C57">
-        <v>0.8858162760734558</v>
+        <v>0.819373607635498</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1018,10 +1018,10 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>4.566248416900635</v>
+        <v>5.543291091918945</v>
       </c>
       <c r="C58">
-        <v>0.8925032615661621</v>
+        <v>0.8376485705375671</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1029,10 +1029,10 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>4.666642189025879</v>
+        <v>5.49190616607666</v>
       </c>
       <c r="C59">
-        <v>0.8863545060157776</v>
+        <v>0.8368971347808838</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1040,10 +1040,10 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>4.577247619628906</v>
+        <v>5.500041484832764</v>
       </c>
       <c r="C60">
-        <v>0.8896925449371338</v>
+        <v>0.8446533679962158</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1051,10 +1051,10 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>4.574824810028076</v>
+        <v>5.811877727508545</v>
       </c>
       <c r="C61">
-        <v>0.8917338848114014</v>
+        <v>0.8048028349876404</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1062,10 +1062,10 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>4.415247917175293</v>
+        <v>5.399606704711914</v>
       </c>
       <c r="C62">
-        <v>0.8989494442939758</v>
+        <v>0.8432849645614624</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1073,10 +1073,10 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>4.34369945526123</v>
+        <v>5.826673984527588</v>
       </c>
       <c r="C63">
-        <v>0.9003224968910217</v>
+        <v>0.8180335164070129</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1084,10 +1084,10 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>4.489430904388428</v>
+        <v>5.551222324371338</v>
       </c>
       <c r="C64">
-        <v>0.8989962339401245</v>
+        <v>0.8374972343444824</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1095,10 +1095,10 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>4.422661781311035</v>
+        <v>5.506695747375488</v>
       </c>
       <c r="C65">
-        <v>0.8983141183853149</v>
+        <v>0.8374452590942383</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1106,10 +1106,10 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>4.537863254547119</v>
+        <v>5.489109039306641</v>
       </c>
       <c r="C66">
-        <v>0.8931149244308472</v>
+        <v>0.8298180103302002</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1117,10 +1117,10 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>4.554316520690918</v>
+        <v>5.504336357116699</v>
       </c>
       <c r="C67">
-        <v>0.894534707069397</v>
+        <v>0.8374220728874207</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1128,10 +1128,10 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>4.536049842834473</v>
+        <v>5.505527019500732</v>
       </c>
       <c r="C68">
-        <v>0.8937167525291443</v>
+        <v>0.8307868838310242</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1139,10 +1139,10 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>4.437792778015137</v>
+        <v>5.322421073913574</v>
       </c>
       <c r="C69">
-        <v>0.8956853151321411</v>
+        <v>0.8502706289291382</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1150,10 +1150,10 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>4.375246524810791</v>
+        <v>5.484179496765137</v>
       </c>
       <c r="C70">
-        <v>0.9018706679344177</v>
+        <v>0.8451113700866699</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1161,10 +1161,10 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>4.546594142913818</v>
+        <v>5.645872116088867</v>
       </c>
       <c r="C71">
-        <v>0.8905628323554993</v>
+        <v>0.8273598551750183</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1172,10 +1172,10 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>4.420035839080811</v>
+        <v>5.427425384521484</v>
       </c>
       <c r="C72">
-        <v>0.8980636596679688</v>
+        <v>0.8432795405387878</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1183,10 +1183,10 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>4.555513381958008</v>
+        <v>5.218438148498535</v>
       </c>
       <c r="C73">
-        <v>0.8919094204902649</v>
+        <v>0.8524907231330872</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1194,10 +1194,10 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>4.45025634765625</v>
+        <v>5.426321983337402</v>
       </c>
       <c r="C74">
-        <v>0.8942368030548096</v>
+        <v>0.8465814590454102</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1205,10 +1205,10 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>4.539854049682617</v>
+        <v>5.373984813690186</v>
       </c>
       <c r="C75">
-        <v>0.8935588002204895</v>
+        <v>0.8444929122924805</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1216,10 +1216,10 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>4.34919548034668</v>
+        <v>5.129755973815918</v>
       </c>
       <c r="C76">
-        <v>0.9007523059844971</v>
+        <v>0.859188437461853</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1227,10 +1227,10 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>4.346072196960449</v>
+        <v>5.152495861053467</v>
       </c>
       <c r="C77">
-        <v>0.9033629894256592</v>
+        <v>0.8567067384719849</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1238,10 +1238,10 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>4.483687877655029</v>
+        <v>5.28340482711792</v>
       </c>
       <c r="C78">
-        <v>0.8963650465011597</v>
+        <v>0.8545277714729309</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1249,10 +1249,10 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>4.509771823883057</v>
+        <v>5.439005851745605</v>
       </c>
       <c r="C79">
-        <v>0.8929692506790161</v>
+        <v>0.8456141948699951</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1260,10 +1260,10 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>4.393011093139648</v>
+        <v>5.321115016937256</v>
       </c>
       <c r="C80">
-        <v>0.9009555578231812</v>
+        <v>0.8465718626976013</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1271,10 +1271,10 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>4.365672588348389</v>
+        <v>5.30781078338623</v>
       </c>
       <c r="C81">
-        <v>0.8964095711708069</v>
+        <v>0.8530145287513733</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1282,10 +1282,10 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>4.427276134490967</v>
+        <v>5.275221824645996</v>
       </c>
       <c r="C82">
-        <v>0.8987305164337158</v>
+        <v>0.8498678207397461</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1293,10 +1293,10 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>4.429571628570557</v>
+        <v>5.360738754272461</v>
       </c>
       <c r="C83">
-        <v>0.89891517162323</v>
+        <v>0.8512598276138306</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1304,10 +1304,10 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>4.490496635437012</v>
+        <v>5.254478931427002</v>
       </c>
       <c r="C84">
-        <v>0.893377423286438</v>
+        <v>0.842096745967865</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1315,10 +1315,10 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>4.306962966918945</v>
+        <v>5.340359210968018</v>
       </c>
       <c r="C85">
-        <v>0.9039168357849121</v>
+        <v>0.8410004377365112</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1326,10 +1326,10 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>4.430452823638916</v>
+        <v>5.078260898590088</v>
       </c>
       <c r="C86">
-        <v>0.8997037410736084</v>
+        <v>0.8642523884773254</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1337,10 +1337,10 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>4.221965789794922</v>
+        <v>5.075554370880127</v>
       </c>
       <c r="C87">
-        <v>0.9049737453460693</v>
+        <v>0.8659154176712036</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1348,10 +1348,10 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>4.352291584014893</v>
+        <v>5.217664241790771</v>
       </c>
       <c r="C88">
-        <v>0.9022148251533508</v>
+        <v>0.8507083654403687</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1359,10 +1359,10 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>4.327961921691895</v>
+        <v>5.018243789672852</v>
       </c>
       <c r="C89">
-        <v>0.9051989912986755</v>
+        <v>0.86647629737854</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1370,10 +1370,10 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>4.582406044006348</v>
+        <v>5.118835926055908</v>
       </c>
       <c r="C90">
-        <v>0.8877905607223511</v>
+        <v>0.8565160632133484</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1381,10 +1381,10 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>4.434141159057617</v>
+        <v>5.136265277862549</v>
       </c>
       <c r="C91">
-        <v>0.8958969712257385</v>
+        <v>0.8609759211540222</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1392,10 +1392,10 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>4.17602014541626</v>
+        <v>5.101777076721191</v>
       </c>
       <c r="C92">
-        <v>0.9075372219085693</v>
+        <v>0.8664219379425049</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1403,10 +1403,10 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>4.317983627319336</v>
+        <v>5.183019161224365</v>
       </c>
       <c r="C93">
-        <v>0.9045441150665283</v>
+        <v>0.8622119426727295</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1414,10 +1414,10 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>4.270481586456299</v>
+        <v>4.970968723297119</v>
       </c>
       <c r="C94">
-        <v>0.9069610834121704</v>
+        <v>0.8668940663337708</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1425,10 +1425,10 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>4.238768577575684</v>
+        <v>5.068518161773682</v>
       </c>
       <c r="C95">
-        <v>0.9075793027877808</v>
+        <v>0.8643868565559387</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1436,10 +1436,10 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>4.362022399902344</v>
+        <v>4.923008918762207</v>
       </c>
       <c r="C96">
-        <v>0.902093768119812</v>
+        <v>0.8696881532669067</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1447,10 +1447,10 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>4.390330791473389</v>
+        <v>5.269438743591309</v>
       </c>
       <c r="C97">
-        <v>0.8991678953170776</v>
+        <v>0.8547347784042358</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1458,10 +1458,10 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>4.381831645965576</v>
+        <v>5.007972717285156</v>
       </c>
       <c r="C98">
-        <v>0.9024683237075806</v>
+        <v>0.8675112128257751</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1469,10 +1469,10 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>4.329264163970947</v>
+        <v>5.032581806182861</v>
       </c>
       <c r="C99">
-        <v>0.9032279253005981</v>
+        <v>0.8707244396209717</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1480,10 +1480,10 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>4.308911323547363</v>
+        <v>4.917586326599121</v>
       </c>
       <c r="C100">
-        <v>0.9021614789962769</v>
+        <v>0.8734118938446045</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1491,10 +1491,10 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>4.361014842987061</v>
+        <v>5.083066940307617</v>
       </c>
       <c r="C101">
-        <v>0.9032437801361084</v>
+        <v>0.8607407212257385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>